<commit_message>
updated database excel file
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="database" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
@@ -31,25 +31,67 @@
     <t xml:space="preserve">Vocab</t>
   </si>
   <si>
-    <t xml:space="preserve">apple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">banana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kiwi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">watermelon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pineapple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pear</t>
+    <t xml:space="preserve">Letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phonemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple, Pear, Banana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A, B, C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I like ___</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/l/ as in lantern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drawing, singing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiwi, Watermelon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D, E, F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I eat ___, I drink ____</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pineapple, strawberry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G, H, I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train, Airplane, Junction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J, K, L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV, Telephone, Remote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M, N, O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xbox, PS4, Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P, Q, R</t>
   </si>
 </sst>
 </file>
@@ -145,17 +187,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.76020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.12755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -168,6 +216,21 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -177,13 +240,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,10 +263,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,10 +280,52 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>